<commit_message>
Update investment xlsx file
</commit_message>
<xml_diff>
--- a/Investment.xlsx
+++ b/Investment.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jonathanwang/Desktop/Workspace/Macroeconomics_data_analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2E779B9-F01C-7A4E-ADD3-EA4EA6E33937}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78F6DB03-0ACB-384D-84B4-4100ADA3535F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="280" yWindow="500" windowWidth="28240" windowHeight="16320" xr2:uid="{1223AC3A-55B8-EF41-849B-C83C4CBB615A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>date</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -55,10 +55,6 @@
   </si>
   <si>
     <t>BTC-USD</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ASML</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -462,10 +458,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B955E768-8098-DE44-8118-79351A92ABE9}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -490,31 +486,26 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="2">
-        <v>44805</v>
+        <v>44593</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C2">
         <v>1000</v>
       </c>
       <c r="D2">
-        <v>657</v>
+        <v>43188</v>
       </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="2">
-        <v>44927</v>
-      </c>
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3">
-        <v>1000</v>
-      </c>
-      <c r="D3">
-        <v>16625</v>
-      </c>
+      <c r="A3" s="2"/>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="2"/>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>